<commit_message>
add Int and LocalDateTime cell parsers
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheet_examples/cell_parsers.xlsx
+++ b/src/test/resources/spreadsheet_examples/cell_parsers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/spreadsheet_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A8ECE1-4D1C-594D-A82D-D299C26F3CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEB2077-4CA9-8347-9B68-E5784E0C0AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{8FC5C0BD-89C0-414B-A5CA-9C6500A5AC53}"/>
+    <workbookView xWindow="8200" yWindow="8600" windowWidth="28040" windowHeight="17440" xr2:uid="{8FC5C0BD-89C0-414B-A5CA-9C6500A5AC53}"/>
   </bookViews>
   <sheets>
     <sheet name="cell_parsers" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>string</t>
   </si>
@@ -67,12 +67,21 @@
   </si>
   <si>
     <t>2.78</t>
+  </si>
+  <si>
+    <t>double_int</t>
+  </si>
+  <si>
+    <t>date_time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -102,11 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,19 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909622B-DAA7-1243-9E83-94FC53503F77}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,15 +470,21 @@
       <c r="H1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>3.1415000000000002</v>
       </c>
       <c r="D2">
@@ -478,8 +496,14 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="5">
+        <v>44542.655358796299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>